<commit_message>
add adj ratio responses
</commit_message>
<xml_diff>
--- a/data-fix/validation/validation_in.xlsx
+++ b/data-fix/validation/validation_in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\data-fix\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BE8031-0B32-428B-9C66-C067BA7441AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68741468-2BC9-40CA-8427-5B3D7D655671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{5213FD81-94F1-4039-B3EE-A60BF91D0DB5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="111">
   <si>
     <t>absolute_yield</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>1m2</t>
+  </si>
+  <si>
+    <t>12r-adj</t>
+  </si>
+  <si>
+    <t>bir-adj</t>
   </si>
 </sst>
 </file>
@@ -732,15 +738,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EB5BFE-6567-4E1D-BACA-FE452495DF60}">
-  <dimension ref="A1:BP7"/>
+  <dimension ref="A1:BR7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:H3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="9.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -748,205 +757,211 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>46</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>47</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>48</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>49</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>50</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>51</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>52</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>53</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BJ1" t="s">
         <v>54</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BK1" t="s">
         <v>55</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BL1" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BM1" t="s">
         <v>57</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BN1" t="s">
         <v>58</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BO1" t="s">
         <v>59</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BP1" t="s">
         <v>60</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BQ1" t="s">
         <v>61</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BR1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.5561679222662956</v>
       </c>
@@ -960,199 +975,205 @@
         <v>2.7311977238097325</v>
       </c>
       <c r="E2">
+        <v>2.7311977238097325</v>
+      </c>
+      <c r="F2">
+        <v>2.7311977238097325</v>
+      </c>
+      <c r="G2">
         <v>0.46397908981411362</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.46397908981411362</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>2.1139666456133774</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>2.1139666456133774</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>6.6875333497431466E-2</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>2.9355956425840789E-2</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>63</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>1.8568131300699</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>1.8435525487492801</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>1.84561453180234</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>96.341138965656199</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>102.01962814978</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>101.352127992856</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>62.093342663304497</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>27.445192114378699</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>37.200000000000003</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>7.7629207827873401</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>3.20729557053575</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>6.3225030101252004</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>94</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>0.112469</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>-3.7032000000000002E-2</v>
       </c>
-      <c r="AA2">
+      <c r="AC2">
         <v>-3.7026999999999997E-2</v>
       </c>
-      <c r="AB2">
+      <c r="AD2">
         <v>-0.218081</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>0.49265900000000001</v>
       </c>
-      <c r="AD2">
+      <c r="AF2">
         <v>-0.17632500000000001</v>
       </c>
-      <c r="AE2">
+      <c r="AG2">
         <v>-0.17619299999999999</v>
       </c>
-      <c r="AF2">
+      <c r="AH2">
         <v>-0.13664899999999999</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>533.56399999999996</v>
       </c>
-      <c r="AH2">
+      <c r="AJ2">
         <v>189.25299999999999</v>
       </c>
-      <c r="AI2">
+      <c r="AK2">
         <v>1297.81</v>
       </c>
-      <c r="AJ2">
+      <c r="AL2">
         <v>-0.25402000000000002</v>
       </c>
-      <c r="AK2">
+      <c r="AM2">
         <v>3.3210000000000003E-2</v>
       </c>
-      <c r="AL2">
+      <c r="AN2">
         <v>180.23969729999999</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>95</v>
       </c>
-      <c r="AN2">
+      <c r="AP2">
         <v>0.19575999999999999</v>
       </c>
-      <c r="AO2">
+      <c r="AQ2">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="AP2">
+      <c r="AR2">
         <v>-2.7101E-2</v>
       </c>
-      <c r="AQ2">
+      <c r="AS2">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="AR2">
+      <c r="AT2">
         <v>0.52158599999999999</v>
       </c>
-      <c r="AS2">
+      <c r="AU2">
         <v>-0.184866</v>
       </c>
-      <c r="AT2">
+      <c r="AV2">
         <v>-0.150033</v>
       </c>
-      <c r="AU2">
+      <c r="AW2">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="AV2">
+      <c r="AX2">
         <v>497.02800000000002</v>
       </c>
-      <c r="AW2">
+      <c r="AY2">
         <v>58.020899999999997</v>
       </c>
-      <c r="AX2">
+      <c r="AZ2">
         <v>1117.57</v>
       </c>
-      <c r="AY2">
+      <c r="BA2">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="AZ2">
+      <c r="BB2">
         <v>-2.409E-2</v>
       </c>
-      <c r="BA2">
+      <c r="BC2">
         <v>137.28036270000001</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BD2" t="s">
         <v>95</v>
       </c>
-      <c r="BC2">
+      <c r="BE2">
         <v>0.19575999999999999</v>
       </c>
-      <c r="BD2">
+      <c r="BF2">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="BE2">
+      <c r="BG2">
         <v>-2.7101E-2</v>
       </c>
-      <c r="BF2">
+      <c r="BH2">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="BG2">
+      <c r="BI2">
         <v>0.52158599999999999</v>
       </c>
-      <c r="BH2">
+      <c r="BJ2">
         <v>-0.184866</v>
       </c>
-      <c r="BI2">
+      <c r="BK2">
         <v>-0.150033</v>
       </c>
-      <c r="BJ2">
+      <c r="BL2">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="BK2">
+      <c r="BM2">
         <v>497.02800000000002</v>
       </c>
-      <c r="BL2">
+      <c r="BN2">
         <v>58.020899999999997</v>
       </c>
-      <c r="BM2">
+      <c r="BO2">
         <v>1117.57</v>
       </c>
-      <c r="BN2">
+      <c r="BP2">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="BO2">
+      <c r="BQ2">
         <v>-2.409E-2</v>
       </c>
-      <c r="BP2">
+      <c r="BR2">
         <v>137.28036270000001</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9.1167325678820248</v>
       </c>
@@ -1160,205 +1181,211 @@
         <v>75</v>
       </c>
       <c r="C3">
+        <v>0.97177560637350935</v>
+      </c>
+      <c r="D3">
         <v>0.70278798737415737</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <v>0.70278798737415737</v>
+      </c>
+      <c r="F3">
         <v>0.97177560637350935</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>-0.17454434423405152</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>-1.4314201644070934E-2</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>-1.5912741076181884</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>-0.13049874831173192</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0.16511373658666006</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>3.6222130101381013E-2</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>64</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>1.8793131724116601</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>1.90204258627402</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>1.91557745862703</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>114.269561589658</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>113.472992085035</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>113.005406354765</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>75.040387449617199</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>33.510381331748803</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>74.599999999999994</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>8.5097539997699592</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>5.2588066191272604</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>8.2152456495596198</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>99</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>0.17913699999999999</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>-4.0078000000000003E-2</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <v>-4.0072000000000003E-2</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>-0.47377799999999998</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>0.41362199999999999</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>-0.17389099999999999</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>-0.17425599999999999</v>
       </c>
-      <c r="AF3">
+      <c r="AH3">
         <v>-2.4944000000000001E-2</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>465.96600000000001</v>
       </c>
-      <c r="AH3">
+      <c r="AJ3">
         <v>154.71700000000001</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>1379.14</v>
       </c>
-      <c r="AJ3">
+      <c r="AL3">
         <v>-0.24607000000000001</v>
       </c>
-      <c r="AK3">
+      <c r="AM3">
         <v>2.155E-2</v>
       </c>
-      <c r="AL3">
+      <c r="AN3">
         <v>167.93422620000001</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AO3" t="s">
         <v>99</v>
       </c>
-      <c r="AN3">
+      <c r="AP3">
         <v>0.17913699999999999</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>-4.0078000000000003E-2</v>
       </c>
-      <c r="AP3">
+      <c r="AR3">
         <v>-4.0072000000000003E-2</v>
       </c>
-      <c r="AQ3">
+      <c r="AS3">
         <v>-0.47377799999999998</v>
       </c>
-      <c r="AR3">
+      <c r="AT3">
         <v>0.41362199999999999</v>
       </c>
-      <c r="AS3">
+      <c r="AU3">
         <v>-0.17389099999999999</v>
       </c>
-      <c r="AT3">
+      <c r="AV3">
         <v>-0.17425599999999999</v>
       </c>
-      <c r="AU3">
+      <c r="AW3">
         <v>-2.4944000000000001E-2</v>
       </c>
-      <c r="AV3">
+      <c r="AX3">
         <v>465.96600000000001</v>
       </c>
-      <c r="AW3">
+      <c r="AY3">
         <v>154.71700000000001</v>
       </c>
-      <c r="AX3">
+      <c r="AZ3">
         <v>1379.14</v>
       </c>
-      <c r="AY3">
+      <c r="BA3">
         <v>-0.24607000000000001</v>
       </c>
-      <c r="AZ3">
+      <c r="BB3">
         <v>2.155E-2</v>
       </c>
-      <c r="BA3">
+      <c r="BC3">
         <v>167.93422620000001</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BD3" t="s">
         <v>100</v>
       </c>
-      <c r="BC3">
+      <c r="BE3">
         <v>0.210537</v>
       </c>
-      <c r="BD3">
+      <c r="BF3">
         <v>-0.18282599999999999</v>
       </c>
-      <c r="BE3">
+      <c r="BG3">
         <v>-2.5245E-2</v>
       </c>
-      <c r="BF3">
+      <c r="BH3">
         <v>-8.1609999999999999E-3</v>
       </c>
-      <c r="BG3">
+      <c r="BI3">
         <v>0.50115699999999996</v>
       </c>
-      <c r="BH3">
+      <c r="BJ3">
         <v>-0.142571</v>
       </c>
-      <c r="BI3">
+      <c r="BK3">
         <v>-0.15087999999999999</v>
       </c>
-      <c r="BJ3">
+      <c r="BL3">
         <v>-0.130694</v>
       </c>
-      <c r="BK3">
+      <c r="BM3">
         <v>524.41399999999999</v>
       </c>
-      <c r="BL3">
+      <c r="BN3">
         <v>65.549800000000005</v>
       </c>
-      <c r="BM3">
+      <c r="BO3">
         <v>1095.94</v>
       </c>
-      <c r="BN3">
+      <c r="BP3">
         <v>-0.20849000000000001</v>
       </c>
-      <c r="BO3">
+      <c r="BQ3">
         <v>-2.1530000000000001E-2</v>
       </c>
-      <c r="BP3">
+      <c r="BR3">
         <v>117.3192696</v>
       </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.9556005164145376</v>
       </c>
@@ -1372,199 +1399,205 @@
         <v>0.85552070700928484</v>
       </c>
       <c r="E4">
+        <v>0.85552070700928484</v>
+      </c>
+      <c r="F4">
+        <v>0.85552070700928484</v>
+      </c>
+      <c r="G4">
         <v>-7.7864554378153927E-2</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>-7.7864554378153927E-2</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>-0.1522719627523057</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>-0.1522719627523057</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>1.8667264290128906E-2</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>1.9091081367020792E-2</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>65</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>1.8936224544507201</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>1.8949749338711499</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>1.8520610141137299</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>117.918449107021</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>110.849296192537</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>108.51763249927799</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>73.581357917434204</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>32.686921954504598</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>67.8</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>7.4404857623436103</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>3.9560121107426101</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>6.5403197959766501</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>101</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>0.15546399999999999</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>-3.7927000000000002E-2</v>
       </c>
-      <c r="AA4">
+      <c r="AC4">
         <v>-3.7895999999999999E-2</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>-0.43332700000000002</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>0.39064500000000002</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>-0.17117199999999999</v>
       </c>
-      <c r="AE4">
+      <c r="AG4">
         <v>-0.17145299999999999</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>6.7978999999999998E-2</v>
       </c>
-      <c r="AG4">
+      <c r="AI4">
         <v>464.04</v>
       </c>
-      <c r="AH4">
+      <c r="AJ4">
         <v>158.369</v>
       </c>
-      <c r="AI4">
+      <c r="AK4">
         <v>1200.6500000000001</v>
       </c>
-      <c r="AJ4">
+      <c r="AL4">
         <v>-0.25013999999999997</v>
       </c>
-      <c r="AK4">
+      <c r="AM4">
         <v>2.3949999999999999E-2</v>
       </c>
-      <c r="AL4">
+      <c r="AN4">
         <v>171.9942159</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AO4" t="s">
         <v>101</v>
       </c>
-      <c r="AN4">
+      <c r="AP4">
         <v>0.15546399999999999</v>
       </c>
-      <c r="AO4">
+      <c r="AQ4">
         <v>-3.7927000000000002E-2</v>
       </c>
-      <c r="AP4">
+      <c r="AR4">
         <v>-3.7895999999999999E-2</v>
       </c>
-      <c r="AQ4">
+      <c r="AS4">
         <v>-0.43332700000000002</v>
       </c>
-      <c r="AR4">
+      <c r="AT4">
         <v>0.39064500000000002</v>
       </c>
-      <c r="AS4">
+      <c r="AU4">
         <v>-0.17117199999999999</v>
       </c>
-      <c r="AT4">
+      <c r="AV4">
         <v>-0.17145299999999999</v>
       </c>
-      <c r="AU4">
+      <c r="AW4">
         <v>6.7978999999999998E-2</v>
       </c>
-      <c r="AV4">
+      <c r="AX4">
         <v>464.04</v>
       </c>
-      <c r="AW4">
+      <c r="AY4">
         <v>158.369</v>
       </c>
-      <c r="AX4">
+      <c r="AZ4">
         <v>1200.6500000000001</v>
       </c>
-      <c r="AY4">
+      <c r="BA4">
         <v>-0.25013999999999997</v>
       </c>
-      <c r="AZ4">
+      <c r="BB4">
         <v>2.3949999999999999E-2</v>
       </c>
-      <c r="BA4">
+      <c r="BC4">
         <v>171.9942159</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BD4" t="s">
         <v>102</v>
       </c>
-      <c r="BC4">
+      <c r="BE4">
         <v>0.203903</v>
       </c>
-      <c r="BD4">
+      <c r="BF4">
         <v>-0.227689</v>
       </c>
-      <c r="BE4">
+      <c r="BG4">
         <v>-0.16625799999999999</v>
       </c>
-      <c r="BF4">
+      <c r="BH4">
         <v>1.6063000000000001E-2</v>
       </c>
-      <c r="BG4">
+      <c r="BI4">
         <v>0.58998300000000004</v>
-      </c>
-      <c r="BH4">
-        <v>-6.2940999999999997E-2</v>
-      </c>
-      <c r="BI4">
-        <v>-6.2940999999999997E-2</v>
       </c>
       <c r="BJ4">
         <v>-6.2940999999999997E-2</v>
       </c>
       <c r="BK4">
+        <v>-6.2940999999999997E-2</v>
+      </c>
+      <c r="BL4">
+        <v>-6.2940999999999997E-2</v>
+      </c>
+      <c r="BM4">
         <v>511.89</v>
       </c>
-      <c r="BL4">
+      <c r="BN4">
         <v>61.433100000000003</v>
       </c>
-      <c r="BM4">
+      <c r="BO4">
         <v>1092.25</v>
       </c>
-      <c r="BN4">
+      <c r="BP4">
         <v>-0.24740000000000001</v>
       </c>
-      <c r="BO4">
+      <c r="BQ4">
         <v>-3.0190000000000002E-2</v>
       </c>
-      <c r="BP4">
+      <c r="BR4">
         <v>136.30144709999999</v>
       </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17.01878492428709</v>
       </c>
@@ -1572,205 +1605,211 @@
         <v>352</v>
       </c>
       <c r="C5">
+        <v>4.4390731260818646</v>
+      </c>
+      <c r="D5">
         <v>0.65509853907386295</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <v>0.65509853907386295</v>
+      </c>
+      <c r="F5">
         <v>4.4390731260818646</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>-0.20838726685066872</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.63229029034203543</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>-3.5464980754915514</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>10.760812461046141</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>2.8837594834960251E-2</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>3.3889134815737435E-3</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>66</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>1.8508149556344</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>1.8769339359710999</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>1.87825530745955</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>106.05218684571</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>106.46566720430501</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>104.721172548957</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>67.019856180771896</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>29.7533761463113</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>48.5</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>7.6925284248122301</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>4.3823070061186904</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>6.8148663930706803</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>96</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>0.153248</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>-0.273613</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AE5">
+      <c r="AG5">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AF5">
+      <c r="AH5">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AG5">
+      <c r="AI5">
         <v>504.39800000000002</v>
       </c>
-      <c r="AH5">
+      <c r="AJ5">
         <v>159.078</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>1213.46</v>
       </c>
-      <c r="AJ5">
+      <c r="AL5">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="AK5">
+      <c r="AM5">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="AL5">
+      <c r="AN5">
         <v>174.29090249999999</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AO5" t="s">
         <v>96</v>
       </c>
-      <c r="AN5">
+      <c r="AP5">
         <v>0.153248</v>
       </c>
-      <c r="AO5">
+      <c r="AQ5">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AP5">
+      <c r="AR5">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AQ5">
+      <c r="AS5">
         <v>-0.273613</v>
       </c>
-      <c r="AR5">
+      <c r="AT5">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AS5">
+      <c r="AU5">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AT5">
+      <c r="AV5">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AU5">
+      <c r="AW5">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AV5">
+      <c r="AX5">
         <v>504.39800000000002</v>
       </c>
-      <c r="AW5">
+      <c r="AY5">
         <v>159.078</v>
       </c>
-      <c r="AX5">
+      <c r="AZ5">
         <v>1213.46</v>
       </c>
-      <c r="AY5">
+      <c r="BA5">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="AZ5">
+      <c r="BB5">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="BA5">
+      <c r="BC5">
         <v>174.29090249999999</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BD5" t="s">
         <v>97</v>
       </c>
-      <c r="BC5">
+      <c r="BE5">
         <v>0.192499</v>
       </c>
-      <c r="BD5">
+      <c r="BF5">
         <v>-2.8559999999999999E-2</v>
       </c>
-      <c r="BE5">
+      <c r="BG5">
         <v>-2.8577999999999999E-2</v>
       </c>
-      <c r="BF5">
+      <c r="BH5">
         <v>-0.19442300000000001</v>
       </c>
-      <c r="BG5">
+      <c r="BI5">
         <v>0.61518899999999999</v>
       </c>
-      <c r="BH5">
+      <c r="BJ5">
         <v>-0.18667</v>
       </c>
-      <c r="BI5">
+      <c r="BK5">
         <v>-0.18692500000000001</v>
       </c>
-      <c r="BJ5">
+      <c r="BL5">
         <v>-0.230076</v>
       </c>
-      <c r="BK5">
+      <c r="BM5">
         <v>523.923</v>
       </c>
-      <c r="BL5">
+      <c r="BN5">
         <v>60.247799999999998</v>
       </c>
-      <c r="BM5">
+      <c r="BO5">
         <v>1062.54</v>
       </c>
-      <c r="BN5">
+      <c r="BP5">
         <v>-0.25189</v>
       </c>
-      <c r="BO5">
+      <c r="BQ5">
         <v>-2.6440000000000002E-2</v>
       </c>
-      <c r="BP5">
+      <c r="BR5">
         <v>141.47212949999999</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6.1892009610592513</v>
       </c>
@@ -1784,199 +1823,205 @@
         <v>3.7349086386076782</v>
       </c>
       <c r="E6">
+        <v>3.7349086386076782</v>
+      </c>
+      <c r="F6">
+        <v>3.7349086386076782</v>
+      </c>
+      <c r="G6">
         <v>0.57760536630161696</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.57760536630161696</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>3.5749156882269482</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>3.5749156882269482</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>0.13796842968809828</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>4.4583599904465102E-2</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>67</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>1.8767439889340201</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>1.84538261615308</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>1.8407903194008799</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>107.899835309827</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>99.799036713283598</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>100.674362787128</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>64.417883073343702</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>28.498714588642201</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>42.5</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>7.7906856888925198</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>3.9768691261210298</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>6.42864299314751</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>103</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>0.137624</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>-3.7663000000000002E-2</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <v>-4.0806000000000002E-2</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>-0.27689200000000003</v>
       </c>
-      <c r="AC6">
+      <c r="AE6">
         <v>0.40879100000000002</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>-0.173319</v>
       </c>
-      <c r="AE6">
+      <c r="AG6">
         <v>-0.16671800000000001</v>
       </c>
-      <c r="AF6">
+      <c r="AH6">
         <v>5.4883000000000001E-2</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>480.26</v>
       </c>
-      <c r="AH6">
+      <c r="AJ6">
         <v>164.738</v>
       </c>
-      <c r="AI6">
+      <c r="AK6">
         <v>1264.95</v>
       </c>
-      <c r="AJ6">
+      <c r="AL6">
         <v>-0.25147999999999998</v>
       </c>
-      <c r="AK6">
+      <c r="AM6">
         <v>2.8500000000000001E-2</v>
       </c>
-      <c r="AL6">
+      <c r="AN6">
         <v>175.6902498</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AO6" t="s">
         <v>95</v>
       </c>
-      <c r="AN6">
+      <c r="AP6">
         <v>0.19575999999999999</v>
       </c>
-      <c r="AO6">
+      <c r="AQ6">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="AP6">
+      <c r="AR6">
         <v>-2.7101E-2</v>
       </c>
-      <c r="AQ6">
+      <c r="AS6">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="AR6">
+      <c r="AT6">
         <v>0.52158599999999999</v>
       </c>
-      <c r="AS6">
+      <c r="AU6">
         <v>-0.184866</v>
       </c>
-      <c r="AT6">
+      <c r="AV6">
         <v>-0.150033</v>
       </c>
-      <c r="AU6">
+      <c r="AW6">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="AV6">
+      <c r="AX6">
         <v>497.02800000000002</v>
       </c>
-      <c r="AW6">
+      <c r="AY6">
         <v>58.020899999999997</v>
       </c>
-      <c r="AX6">
+      <c r="AZ6">
         <v>1117.57</v>
       </c>
-      <c r="AY6">
+      <c r="BA6">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="AZ6">
+      <c r="BB6">
         <v>-2.409E-2</v>
       </c>
-      <c r="BA6">
+      <c r="BC6">
         <v>137.28036270000001</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BD6" t="s">
         <v>95</v>
       </c>
-      <c r="BC6">
+      <c r="BE6">
         <v>0.19575999999999999</v>
       </c>
-      <c r="BD6">
+      <c r="BF6">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="BE6">
+      <c r="BG6">
         <v>-2.7101E-2</v>
       </c>
-      <c r="BF6">
+      <c r="BH6">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="BG6">
+      <c r="BI6">
         <v>0.52158599999999999</v>
       </c>
-      <c r="BH6">
+      <c r="BJ6">
         <v>-0.184866</v>
       </c>
-      <c r="BI6">
+      <c r="BK6">
         <v>-0.150033</v>
       </c>
-      <c r="BJ6">
+      <c r="BL6">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="BK6">
+      <c r="BM6">
         <v>497.02800000000002</v>
       </c>
-      <c r="BL6">
+      <c r="BN6">
         <v>58.020899999999997</v>
       </c>
-      <c r="BM6">
+      <c r="BO6">
         <v>1117.57</v>
       </c>
-      <c r="BN6">
+      <c r="BP6">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="BO6">
+      <c r="BQ6">
         <v>-2.409E-2</v>
       </c>
-      <c r="BP6">
+      <c r="BR6">
         <v>137.28036270000001</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6.4225476710000002</v>
       </c>
@@ -1984,201 +2029,207 @@
         <v>354</v>
       </c>
       <c r="C7">
+        <v>4.0191051336105357</v>
+      </c>
+      <c r="D7">
         <v>6.3219039441309244E-2</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <v>6.3219039441309244E-2</v>
+      </c>
+      <c r="F7">
         <v>4.0191051336105357</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>-0.8810799334922953</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.60152259282098697</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>-5.6587778752409301</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>3.8633075278665681</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>7.9161313999999997E-2</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>2.4651063000000001E-2</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>68</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>1.8579539819999999</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>1.876727737</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>1.877293264</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>108.4757733</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>110.22450980000001</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>105.9976198</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>69.303228919999995</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>30.752714340000001</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>52.1</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>7.88372662</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>4.8875613429999998</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>7.6535070090000001</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>96</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>0.153248</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AA7">
+      <c r="AC7">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>-0.273613</v>
       </c>
-      <c r="AC7">
+      <c r="AE7">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AE7">
+      <c r="AG7">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AF7">
+      <c r="AH7">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>504.39800000000002</v>
       </c>
-      <c r="AH7">
+      <c r="AJ7">
         <v>159.078</v>
       </c>
-      <c r="AI7">
+      <c r="AK7">
         <v>1213.46</v>
       </c>
-      <c r="AJ7">
+      <c r="AL7">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="AK7">
+      <c r="AM7">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="AL7">
+      <c r="AN7">
         <v>174.29090249999999</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AO7" t="s">
         <v>96</v>
       </c>
-      <c r="AN7">
+      <c r="AP7">
         <v>0.153248</v>
       </c>
-      <c r="AO7">
+      <c r="AQ7">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AP7">
+      <c r="AR7">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7">
         <v>-0.273613</v>
       </c>
-      <c r="AR7">
+      <c r="AT7">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AS7">
+      <c r="AU7">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AT7">
+      <c r="AV7">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AU7">
+      <c r="AW7">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AV7">
+      <c r="AX7">
         <v>504.39800000000002</v>
       </c>
-      <c r="AW7">
+      <c r="AY7">
         <v>159.078</v>
       </c>
-      <c r="AX7">
+      <c r="AZ7">
         <v>1213.46</v>
       </c>
-      <c r="AY7">
+      <c r="BA7">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="AZ7">
+      <c r="BB7">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="BA7">
+      <c r="BC7">
         <v>174.29090249999999</v>
       </c>
-      <c r="BB7" t="s">
+      <c r="BD7" t="s">
         <v>98</v>
       </c>
-      <c r="BC7">
+      <c r="BE7">
         <v>0.17724599999999999</v>
       </c>
-      <c r="BD7">
+      <c r="BF7">
         <v>-2.9998E-2</v>
       </c>
-      <c r="BE7">
+      <c r="BG7">
         <v>-3.0117000000000001E-2</v>
       </c>
-      <c r="BF7">
+      <c r="BH7">
         <v>-0.22006999999999999</v>
       </c>
-      <c r="BG7">
+      <c r="BI7">
         <v>0.61323799999999995</v>
       </c>
-      <c r="BH7">
+      <c r="BJ7">
         <v>-0.18851399999999999</v>
       </c>
-      <c r="BI7">
+      <c r="BK7">
         <v>-0.18893499999999999</v>
       </c>
-      <c r="BJ7">
+      <c r="BL7">
         <v>-0.30469200000000002</v>
       </c>
-      <c r="BK7">
+      <c r="BM7">
         <v>538.20899999999995</v>
       </c>
-      <c r="BL7">
+      <c r="BN7">
         <v>64.740600000000001</v>
       </c>
-      <c r="BM7">
+      <c r="BO7">
         <v>1070.8900000000001</v>
       </c>
-      <c r="BN7">
+      <c r="BP7">
         <v>-0.24277000000000001</v>
       </c>
-      <c r="BO7">
+      <c r="BQ7">
         <v>-2.3910000000000001E-2</v>
       </c>
-      <c r="BP7">
+      <c r="BR7">
         <v>137.33683859999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add kennard stone splitting
</commit_message>
<xml_diff>
--- a/data-fix/validation/validation_in.xlsx
+++ b/data-fix/validation/validation_in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\data-fix\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68741468-2BC9-40CA-8427-5B3D7D655671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F71D22-6B84-4DB2-9948-ECBAF20C509A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{5213FD81-94F1-4039-B3EE-A60BF91D0DB5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="112">
   <si>
     <t>absolute_yield</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>bir-adj</t>
+  </si>
+  <si>
+    <t>inv-12r-adj</t>
   </si>
 </sst>
 </file>
@@ -738,18 +741,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EB5BFE-6567-4E1D-BACA-FE452495DF60}">
-  <dimension ref="A1:BR7"/>
+  <dimension ref="A1:BS7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="9.25" customWidth="1"/>
+    <col min="2" max="5" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -757,211 +760,214 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>34</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>35</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>36</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>37</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>38</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>39</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>41</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>42</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>43</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>44</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>45</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>46</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>47</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>48</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>49</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>50</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>51</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>52</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>53</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>54</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>55</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>56</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>57</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>58</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>59</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>60</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>61</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.5561679222662956</v>
       </c>
@@ -969,7 +975,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>2.7311977238097325</v>
+        <v>0.36613973103532965</v>
       </c>
       <c r="D2">
         <v>2.7311977238097325</v>
@@ -981,199 +987,202 @@
         <v>2.7311977238097325</v>
       </c>
       <c r="G2">
-        <v>0.46397908981411362</v>
+        <v>2.7311977238097325</v>
       </c>
       <c r="H2">
         <v>0.46397908981411362</v>
       </c>
       <c r="I2">
-        <v>2.1139666456133774</v>
+        <v>0.46397908981411362</v>
       </c>
       <c r="J2">
         <v>2.1139666456133774</v>
       </c>
       <c r="K2">
+        <v>2.1139666456133774</v>
+      </c>
+      <c r="L2">
         <v>6.6875333497431466E-2</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2.9355956425840789E-2</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>63</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1.8568131300699</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1.8435525487492801</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1.84561453180234</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>96.341138965656199</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>102.01962814978</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>101.352127992856</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>62.093342663304497</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>27.445192114378699</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>37.200000000000003</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>7.7629207827873401</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>3.20729557053575</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>6.3225030101252004</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>94</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>0.112469</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>-3.7032000000000002E-2</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>-3.7026999999999997E-2</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>-0.218081</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>0.49265900000000001</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>-0.17632500000000001</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>-0.17619299999999999</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>-0.13664899999999999</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>533.56399999999996</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>189.25299999999999</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <v>1297.81</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>-0.25402000000000002</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>3.3210000000000003E-2</v>
       </c>
-      <c r="AN2">
+      <c r="AO2">
         <v>180.23969729999999</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>95</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>0.19575999999999999</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>-2.7101E-2</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="AT2">
+      <c r="AU2">
         <v>0.52158599999999999</v>
       </c>
-      <c r="AU2">
+      <c r="AV2">
         <v>-0.184866</v>
       </c>
-      <c r="AV2">
+      <c r="AW2">
         <v>-0.150033</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <v>497.02800000000002</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <v>58.020899999999997</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <v>1117.57</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="BB2">
+      <c r="BC2">
         <v>-2.409E-2</v>
       </c>
-      <c r="BC2">
+      <c r="BD2">
         <v>137.28036270000001</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>95</v>
       </c>
-      <c r="BE2">
+      <c r="BF2">
         <v>0.19575999999999999</v>
       </c>
-      <c r="BF2">
+      <c r="BG2">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="BG2">
+      <c r="BH2">
         <v>-2.7101E-2</v>
       </c>
-      <c r="BH2">
+      <c r="BI2">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="BI2">
+      <c r="BJ2">
         <v>0.52158599999999999</v>
       </c>
-      <c r="BJ2">
+      <c r="BK2">
         <v>-0.184866</v>
       </c>
-      <c r="BK2">
+      <c r="BL2">
         <v>-0.150033</v>
       </c>
-      <c r="BL2">
+      <c r="BM2">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <v>497.02800000000002</v>
       </c>
-      <c r="BN2">
+      <c r="BO2">
         <v>58.020899999999997</v>
       </c>
-      <c r="BO2">
+      <c r="BP2">
         <v>1117.57</v>
       </c>
-      <c r="BP2">
+      <c r="BQ2">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="BQ2">
+      <c r="BR2">
         <v>-2.409E-2</v>
       </c>
-      <c r="BR2">
+      <c r="BS2">
         <v>137.28036270000001</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9.1167325678820248</v>
       </c>
@@ -1181,211 +1190,214 @@
         <v>75</v>
       </c>
       <c r="C3">
+        <v>1.029044147065822</v>
+      </c>
+      <c r="D3">
         <v>0.97177560637350935</v>
-      </c>
-      <c r="D3">
-        <v>0.70278798737415737</v>
       </c>
       <c r="E3">
         <v>0.70278798737415737</v>
       </c>
       <c r="F3">
+        <v>0.70278798737415737</v>
+      </c>
+      <c r="G3">
         <v>0.97177560637350935</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>-0.17454434423405152</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>-1.4314201644070934E-2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>-1.5912741076181884</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>-0.13049874831173192</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.16511373658666006</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>3.6222130101381013E-2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>64</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1.8793131724116601</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>1.90204258627402</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1.91557745862703</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>114.269561589658</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>113.472992085035</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>113.005406354765</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>75.040387449617199</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>33.510381331748803</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>74.599999999999994</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>8.5097539997699592</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>5.2588066191272604</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>8.2152456495596198</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>99</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>0.17913699999999999</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>-4.0078000000000003E-2</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>-4.0072000000000003E-2</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>-0.47377799999999998</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>0.41362199999999999</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>-0.17389099999999999</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>-0.17425599999999999</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>-2.4944000000000001E-2</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>465.96600000000001</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>154.71700000000001</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>1379.14</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>-0.24607000000000001</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>2.155E-2</v>
       </c>
-      <c r="AN3">
+      <c r="AO3">
         <v>167.93422620000001</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>99</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>0.17913699999999999</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>-4.0078000000000003E-2</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>-4.0072000000000003E-2</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>-0.47377799999999998</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>0.41362199999999999</v>
       </c>
-      <c r="AU3">
+      <c r="AV3">
         <v>-0.17389099999999999</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>-0.17425599999999999</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>-2.4944000000000001E-2</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>465.96600000000001</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>154.71700000000001</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>1379.14</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>-0.24607000000000001</v>
       </c>
-      <c r="BB3">
+      <c r="BC3">
         <v>2.155E-2</v>
       </c>
-      <c r="BC3">
+      <c r="BD3">
         <v>167.93422620000001</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BE3" t="s">
         <v>100</v>
       </c>
-      <c r="BE3">
+      <c r="BF3">
         <v>0.210537</v>
       </c>
-      <c r="BF3">
+      <c r="BG3">
         <v>-0.18282599999999999</v>
       </c>
-      <c r="BG3">
+      <c r="BH3">
         <v>-2.5245E-2</v>
       </c>
-      <c r="BH3">
+      <c r="BI3">
         <v>-8.1609999999999999E-3</v>
       </c>
-      <c r="BI3">
+      <c r="BJ3">
         <v>0.50115699999999996</v>
       </c>
-      <c r="BJ3">
+      <c r="BK3">
         <v>-0.142571</v>
       </c>
-      <c r="BK3">
+      <c r="BL3">
         <v>-0.15087999999999999</v>
       </c>
-      <c r="BL3">
+      <c r="BM3">
         <v>-0.130694</v>
       </c>
-      <c r="BM3">
+      <c r="BN3">
         <v>524.41399999999999</v>
       </c>
-      <c r="BN3">
+      <c r="BO3">
         <v>65.549800000000005</v>
       </c>
-      <c r="BO3">
+      <c r="BP3">
         <v>1095.94</v>
       </c>
-      <c r="BP3">
+      <c r="BQ3">
         <v>-0.20849000000000001</v>
       </c>
-      <c r="BQ3">
+      <c r="BR3">
         <v>-2.1530000000000001E-2</v>
       </c>
-      <c r="BR3">
+      <c r="BS3">
         <v>117.3192696</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.9556005164145376</v>
       </c>
@@ -1393,7 +1405,7 @@
         <v>351</v>
       </c>
       <c r="C4">
-        <v>0.85552070700928484</v>
+        <v>1.1688787796800191</v>
       </c>
       <c r="D4">
         <v>0.85552070700928484</v>
@@ -1405,172 +1417,172 @@
         <v>0.85552070700928484</v>
       </c>
       <c r="G4">
-        <v>-7.7864554378153927E-2</v>
+        <v>0.85552070700928484</v>
       </c>
       <c r="H4">
         <v>-7.7864554378153927E-2</v>
       </c>
       <c r="I4">
-        <v>-0.1522719627523057</v>
+        <v>-7.7864554378153927E-2</v>
       </c>
       <c r="J4">
         <v>-0.1522719627523057</v>
       </c>
       <c r="K4">
+        <v>-0.1522719627523057</v>
+      </c>
+      <c r="L4">
         <v>1.8667264290128906E-2</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1.9091081367020792E-2</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>65</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1.8936224544507201</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1.8949749338711499</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>1.8520610141137299</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>117.918449107021</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>110.849296192537</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>108.51763249927799</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>73.581357917434204</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>32.686921954504598</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>67.8</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>7.4404857623436103</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>3.9560121107426101</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>6.5403197959766501</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>101</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>0.15546399999999999</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>-3.7927000000000002E-2</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>-3.7895999999999999E-2</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>-0.43332700000000002</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>0.39064500000000002</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>-0.17117199999999999</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>-0.17145299999999999</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>6.7978999999999998E-2</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>464.04</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>158.369</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>1200.6500000000001</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>-0.25013999999999997</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>2.3949999999999999E-2</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>171.9942159</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AP4" t="s">
         <v>101</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>0.15546399999999999</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>-3.7927000000000002E-2</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>-3.7895999999999999E-2</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>-0.43332700000000002</v>
       </c>
-      <c r="AT4">
+      <c r="AU4">
         <v>0.39064500000000002</v>
       </c>
-      <c r="AU4">
+      <c r="AV4">
         <v>-0.17117199999999999</v>
       </c>
-      <c r="AV4">
+      <c r="AW4">
         <v>-0.17145299999999999</v>
       </c>
-      <c r="AW4">
+      <c r="AX4">
         <v>6.7978999999999998E-2</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>464.04</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>158.369</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <v>1200.6500000000001</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>-0.25013999999999997</v>
       </c>
-      <c r="BB4">
+      <c r="BC4">
         <v>2.3949999999999999E-2</v>
       </c>
-      <c r="BC4">
+      <c r="BD4">
         <v>171.9942159</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BE4" t="s">
         <v>102</v>
       </c>
-      <c r="BE4">
+      <c r="BF4">
         <v>0.203903</v>
       </c>
-      <c r="BF4">
+      <c r="BG4">
         <v>-0.227689</v>
       </c>
-      <c r="BG4">
+      <c r="BH4">
         <v>-0.16625799999999999</v>
       </c>
-      <c r="BH4">
+      <c r="BI4">
         <v>1.6063000000000001E-2</v>
       </c>
-      <c r="BI4">
+      <c r="BJ4">
         <v>0.58998300000000004</v>
-      </c>
-      <c r="BJ4">
-        <v>-6.2940999999999997E-2</v>
       </c>
       <c r="BK4">
         <v>-6.2940999999999997E-2</v>
@@ -1579,25 +1591,28 @@
         <v>-6.2940999999999997E-2</v>
       </c>
       <c r="BM4">
+        <v>-6.2940999999999997E-2</v>
+      </c>
+      <c r="BN4">
         <v>511.89</v>
       </c>
-      <c r="BN4">
+      <c r="BO4">
         <v>61.433100000000003</v>
       </c>
-      <c r="BO4">
+      <c r="BP4">
         <v>1092.25</v>
       </c>
-      <c r="BP4">
+      <c r="BQ4">
         <v>-0.24740000000000001</v>
       </c>
-      <c r="BQ4">
+      <c r="BR4">
         <v>-3.0190000000000002E-2</v>
       </c>
-      <c r="BR4">
+      <c r="BS4">
         <v>136.30144709999999</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17.01878492428709</v>
       </c>
@@ -1605,211 +1620,214 @@
         <v>352</v>
       </c>
       <c r="C5">
+        <v>0.22527225202136897</v>
+      </c>
+      <c r="D5">
         <v>4.4390731260818646</v>
-      </c>
-      <c r="D5">
-        <v>0.65509853907386295</v>
       </c>
       <c r="E5">
         <v>0.65509853907386295</v>
       </c>
       <c r="F5">
+        <v>0.65509853907386295</v>
+      </c>
+      <c r="G5">
         <v>4.4390731260818646</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>-0.20838726685066872</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.63229029034203543</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>-3.5464980754915514</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10.760812461046141</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2.8837594834960251E-2</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>3.3889134815737435E-3</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>66</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>1.8508149556344</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>1.8769339359710999</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>1.87825530745955</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>106.05218684571</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>106.46566720430501</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>104.721172548957</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>67.019856180771896</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>29.7533761463113</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>48.5</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>7.6925284248122301</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>4.3823070061186904</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>6.8148663930706803</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>96</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>0.153248</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>-0.273613</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>504.39800000000002</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>159.078</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>1213.46</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>174.29090249999999</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>96</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>0.153248</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>-0.273613</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AU5">
+      <c r="AV5">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AV5">
+      <c r="AW5">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>504.39800000000002</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>159.078</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>1213.46</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="BB5">
+      <c r="BC5">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <v>174.29090249999999</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BE5" t="s">
         <v>97</v>
       </c>
-      <c r="BE5">
+      <c r="BF5">
         <v>0.192499</v>
       </c>
-      <c r="BF5">
+      <c r="BG5">
         <v>-2.8559999999999999E-2</v>
       </c>
-      <c r="BG5">
+      <c r="BH5">
         <v>-2.8577999999999999E-2</v>
       </c>
-      <c r="BH5">
+      <c r="BI5">
         <v>-0.19442300000000001</v>
       </c>
-      <c r="BI5">
+      <c r="BJ5">
         <v>0.61518899999999999</v>
       </c>
-      <c r="BJ5">
+      <c r="BK5">
         <v>-0.18667</v>
       </c>
-      <c r="BK5">
+      <c r="BL5">
         <v>-0.18692500000000001</v>
       </c>
-      <c r="BL5">
+      <c r="BM5">
         <v>-0.230076</v>
       </c>
-      <c r="BM5">
+      <c r="BN5">
         <v>523.923</v>
       </c>
-      <c r="BN5">
+      <c r="BO5">
         <v>60.247799999999998</v>
       </c>
-      <c r="BO5">
+      <c r="BP5">
         <v>1062.54</v>
       </c>
-      <c r="BP5">
+      <c r="BQ5">
         <v>-0.25189</v>
       </c>
-      <c r="BQ5">
+      <c r="BR5">
         <v>-2.6440000000000002E-2</v>
       </c>
-      <c r="BR5">
+      <c r="BS5">
         <v>141.47212949999999</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6.1892009610592513</v>
       </c>
@@ -1817,7 +1835,7 @@
         <v>353</v>
       </c>
       <c r="C6">
-        <v>3.7349086386076782</v>
+        <v>0.26774416639352816</v>
       </c>
       <c r="D6">
         <v>3.7349086386076782</v>
@@ -1829,199 +1847,202 @@
         <v>3.7349086386076782</v>
       </c>
       <c r="G6">
-        <v>0.57760536630161696</v>
+        <v>3.7349086386076782</v>
       </c>
       <c r="H6">
         <v>0.57760536630161696</v>
       </c>
       <c r="I6">
-        <v>3.5749156882269482</v>
+        <v>0.57760536630161696</v>
       </c>
       <c r="J6">
         <v>3.5749156882269482</v>
       </c>
       <c r="K6">
+        <v>3.5749156882269482</v>
+      </c>
+      <c r="L6">
         <v>0.13796842968809828</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>4.4583599904465102E-2</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>67</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>1.8767439889340201</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>1.84538261615308</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>1.8407903194008799</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>107.899835309827</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>99.799036713283598</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>100.674362787128</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>64.417883073343702</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>28.498714588642201</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>42.5</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>7.7906856888925198</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>3.9768691261210298</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>6.42864299314751</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>103</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>0.137624</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>-3.7663000000000002E-2</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>-4.0806000000000002E-2</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>-0.27689200000000003</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>0.40879100000000002</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>-0.173319</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>-0.16671800000000001</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>5.4883000000000001E-2</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>480.26</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>164.738</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>1264.95</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>-0.25147999999999998</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>2.8500000000000001E-2</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>175.6902498</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>95</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>0.19575999999999999</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>-2.7101E-2</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>0.52158599999999999</v>
       </c>
-      <c r="AU6">
+      <c r="AV6">
         <v>-0.184866</v>
       </c>
-      <c r="AV6">
+      <c r="AW6">
         <v>-0.150033</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>497.02800000000002</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>58.020899999999997</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>1117.57</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="BB6">
+      <c r="BC6">
         <v>-2.409E-2</v>
       </c>
-      <c r="BC6">
+      <c r="BD6">
         <v>137.28036270000001</v>
       </c>
-      <c r="BD6" t="s">
+      <c r="BE6" t="s">
         <v>95</v>
       </c>
-      <c r="BE6">
+      <c r="BF6">
         <v>0.19575999999999999</v>
       </c>
-      <c r="BF6">
+      <c r="BG6">
         <v>-1.7198000000000001E-2</v>
       </c>
-      <c r="BG6">
+      <c r="BH6">
         <v>-2.7101E-2</v>
       </c>
-      <c r="BH6">
+      <c r="BI6">
         <v>-0.15559300000000001</v>
       </c>
-      <c r="BI6">
+      <c r="BJ6">
         <v>0.52158599999999999</v>
       </c>
-      <c r="BJ6">
+      <c r="BK6">
         <v>-0.184866</v>
       </c>
-      <c r="BK6">
+      <c r="BL6">
         <v>-0.150033</v>
       </c>
-      <c r="BL6">
+      <c r="BM6">
         <v>-8.6227999999999999E-2</v>
       </c>
-      <c r="BM6">
+      <c r="BN6">
         <v>497.02800000000002</v>
       </c>
-      <c r="BN6">
+      <c r="BO6">
         <v>58.020899999999997</v>
       </c>
-      <c r="BO6">
+      <c r="BP6">
         <v>1117.57</v>
       </c>
-      <c r="BP6">
+      <c r="BQ6">
         <v>-0.24285999999999999</v>
       </c>
-      <c r="BQ6">
+      <c r="BR6">
         <v>-2.409E-2</v>
       </c>
-      <c r="BR6">
+      <c r="BS6">
         <v>137.28036270000001</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6.4225476710000002</v>
       </c>
@@ -2029,207 +2050,210 @@
         <v>354</v>
       </c>
       <c r="C7">
+        <v>0.24881160525941676</v>
+      </c>
+      <c r="D7">
         <v>4.0191051336105357</v>
-      </c>
-      <c r="D7">
-        <v>6.3219039441309244E-2</v>
       </c>
       <c r="E7">
         <v>6.3219039441309244E-2</v>
       </c>
       <c r="F7">
+        <v>6.3219039441309244E-2</v>
+      </c>
+      <c r="G7">
         <v>4.0191051336105357</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>-0.8810799334922953</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.60152259282098697</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>-5.6587778752409301</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>3.8633075278665681</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>7.9161313999999997E-2</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>2.4651063000000001E-2</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>68</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>1.8579539819999999</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>1.876727737</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>1.877293264</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>108.4757733</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>110.22450980000001</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>105.9976198</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>69.303228919999995</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>30.752714340000001</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>52.1</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>7.88372662</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>4.8875613429999998</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>7.6535070090000001</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>96</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>0.153248</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AD7">
+      <c r="AE7">
         <v>-0.273613</v>
       </c>
-      <c r="AE7">
+      <c r="AF7">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AG7">
+      <c r="AH7">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AH7">
+      <c r="AI7">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AI7">
+      <c r="AJ7">
         <v>504.39800000000002</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <v>159.078</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>1213.46</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="AN7">
+      <c r="AO7">
         <v>174.29090249999999</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>96</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>0.153248</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>-3.7562999999999999E-2</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>-3.7512999999999998E-2</v>
       </c>
-      <c r="AS7">
+      <c r="AT7">
         <v>-0.273613</v>
       </c>
-      <c r="AT7">
+      <c r="AU7">
         <v>0.43281799999999998</v>
       </c>
-      <c r="AU7">
+      <c r="AV7">
         <v>-0.18011099999999999</v>
       </c>
-      <c r="AV7">
+      <c r="AW7">
         <v>-0.18074100000000001</v>
       </c>
-      <c r="AW7">
+      <c r="AX7">
         <v>3.7199999999999999E-4</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <v>504.39800000000002</v>
       </c>
-      <c r="AY7">
+      <c r="AZ7">
         <v>159.078</v>
       </c>
-      <c r="AZ7">
+      <c r="BA7">
         <v>1213.46</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>-0.25091000000000002</v>
       </c>
-      <c r="BB7">
+      <c r="BC7">
         <v>2.6839999999999999E-2</v>
       </c>
-      <c r="BC7">
+      <c r="BD7">
         <v>174.29090249999999</v>
       </c>
-      <c r="BD7" t="s">
+      <c r="BE7" t="s">
         <v>98</v>
       </c>
-      <c r="BE7">
+      <c r="BF7">
         <v>0.17724599999999999</v>
       </c>
-      <c r="BF7">
+      <c r="BG7">
         <v>-2.9998E-2</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <v>-3.0117000000000001E-2</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <v>-0.22006999999999999</v>
       </c>
-      <c r="BI7">
+      <c r="BJ7">
         <v>0.61323799999999995</v>
       </c>
-      <c r="BJ7">
+      <c r="BK7">
         <v>-0.18851399999999999</v>
       </c>
-      <c r="BK7">
+      <c r="BL7">
         <v>-0.18893499999999999</v>
       </c>
-      <c r="BL7">
+      <c r="BM7">
         <v>-0.30469200000000002</v>
       </c>
-      <c r="BM7">
+      <c r="BN7">
         <v>538.20899999999995</v>
       </c>
-      <c r="BN7">
+      <c r="BO7">
         <v>64.740600000000001</v>
       </c>
-      <c r="BO7">
+      <c r="BP7">
         <v>1070.8900000000001</v>
       </c>
-      <c r="BP7">
+      <c r="BQ7">
         <v>-0.24277000000000001</v>
       </c>
-      <c r="BQ7">
+      <c r="BR7">
         <v>-2.3910000000000001E-2</v>
       </c>
-      <c r="BR7">
+      <c r="BS7">
         <v>137.33683859999999</v>
       </c>
     </row>

</xml_diff>